<commit_message>
mock serial comm and new mode
</commit_message>
<xml_diff>
--- a/6a679c33.xlsx
+++ b/6a679c33.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -366,30 +366,35 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>AV Delay</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>Atrial Amplitude</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Atrial Pulse Width</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Ventricular Amplitude</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Ventricular Pulse Width</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>VRP</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>ARP</t>
         </is>
@@ -408,14 +413,14 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>70</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>1.2</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>1.3</t>
-        </is>
-      </c>
       <c r="E2" t="inlineStr">
         <is>
           <t>1.2</t>
@@ -423,17 +428,22 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>1.4</t>
+          <t>1.2</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>187</t>
+          <t>1.2</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>200</t>
+          <t>150</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>150</t>
         </is>
       </c>
     </row>

</xml_diff>